<commit_message>
[Lab 8] Little changes
</commit_message>
<xml_diff>
--- a/Lab8/Графики.xlsx
+++ b/Lab8/Графики.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Univer\Sec\Lab8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9175E54A-3B68-45BE-8ABB-FB2200243CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F8EB29-75AE-47BB-8F57-E6B53378D033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="594" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -2023,9 +2023,509 @@
               <a:rPr lang="en-US"/>
               <a:t>RSA</a:t>
             </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ASCII RSA ENC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EA6A-478C-8B47-945597916391}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RSA ASCII DEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4000000000000003E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EA6A-478C-8B47-945597916391}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>RSA Base64 ENC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.1000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EA6A-478C-8B47-945597916391}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>RSA Base64 DEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3999999999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EA6A-478C-8B47-945597916391}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1518924367"/>
+        <c:axId val="1518923535"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1518924367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518923535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1518923535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518924367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> and El-Gamal, s</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>El-Gamal</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -2070,21 +2570,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Compare!$A$1:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>RSA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ASCII</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Enc</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>ElGamal Base64 DEC</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2100,33 +2586,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Compare!$A$4:$A$12</c:f>
+              <c:f>Compare!$E$10:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.12E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.49E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.1000000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.9000000000000008E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.8999999999999999E-3</c:v>
+                  <c:v>1.1900000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2134,7 +2605,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-618F-449F-936C-8BC21C139C15}"/>
+              <c16:uniqueId val="{00000000-B605-48FA-A163-78280C79BD30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2142,21 +2613,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Compare!$B$1:$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>RSA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ASCII</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dec</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>ElGamal ASCII DEC</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2172,30 +2629,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Compare!$B$4:$B$12</c:f>
+              <c:f>Compare!$E$4:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0999999999999999E-3</c:v>
+                  <c:v>9.1000000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1000000000000003E-3</c:v>
+                  <c:v>1.32E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4000000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.7000000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.3999999999999995E-3</c:v>
+                  <c:v>1.09E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2203,7 +2648,50 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-618F-449F-936C-8BC21C139C15}"/>
+              <c16:uniqueId val="{00000001-B605-48FA-A163-78280C79BD30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ElGamal Base64 ENC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.4999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0200000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B605-48FA-A163-78280C79BD30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2211,21 +2699,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Compare!$D$1:$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>El-Gamal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ASCII</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Enc</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>ElGamal ASCII ENC</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2241,10 +2715,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Compare!$D$4:$D$12</c:f>
+              <c:f>Compare!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>8.6E-3</c:v>
                 </c:pt>
@@ -2253,21 +2727,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.4999999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.4999999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.35E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0200000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2275,76 +2734,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-618F-449F-936C-8BC21C139C15}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Compare!$E$1:$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>El-Gamal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ASCII</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dec</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Compare!$E$4:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>9.1000000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.32E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.09E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.12E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.49E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1900000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-618F-449F-936C-8BC21C139C15}"/>
+              <c16:uniqueId val="{00000003-B605-48FA-A163-78280C79BD30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2357,83 +2747,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1694588560"/>
-        <c:axId val="1694590224"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Compare!$C$1:$C$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>RSA</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>ASCII</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Dec</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Compare!$C$4:$C$12</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-618F-449F-936C-8BC21C139C15}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="1518924367"/>
+        <c:axId val="1518923535"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1694588560"/>
+        <c:axId val="1518924367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2470,7 +2793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694590224"/>
+        <c:crossAx val="1518923535"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2478,7 +2801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1694590224"/>
+        <c:axId val="1518923535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,6 +2821,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2529,7 +2907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694588560"/>
+        <c:crossAx val="1518924367"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2574,6 +2952,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2591,6 +2976,590 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RSA</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>и </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>El-Gamal</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ASCII RSA ENC</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RSA ASCII DEC</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4000000000000003E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>RSA Base64 ENC</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.1000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>RSA Base64 DEC</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3999999999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>ElGamal Base64 DEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.12E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.49E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1900000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>ElGamal ASCII DEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$E$4:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.1000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.09E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>ElGamal Base64 ENC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.4999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0200000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>ElGamal ASCII ENC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Compare!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4999999999999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-D4C9-4AEB-BEF4-D4ED21B78AC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1518924367"/>
+        <c:axId val="1518923535"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1518924367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518923535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1518923535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518924367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2849,6 +3818,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5430,6 +6439,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6144,23 +7669,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
+        <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FA7547-D77C-48DF-9E15-19C40EA9AC2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2BB591F-1E6E-43F2-9BAD-B0D129868019}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6173,6 +7698,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B05EA8B9-9607-4DB9-8723-C4B564C79984}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771FDFBA-D355-413D-9BE5-636946B62A7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6697,8 +8298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E85247F-CE58-4CF9-B36B-7DA0877DCEC4}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>